<commit_message>
Sesuaikan format upload dan seeder
</commit_message>
<xml_diff>
--- a/storage/app/public/template_upload/Format_Upload_AKI_&_AKB.xlsx
+++ b/storage/app/public/template_upload/Format_Upload_AKI_&_AKB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\OpenDK\storage\app\public\template_upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenDesa\OpenDK\storage\app\public\template_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD26F4E-082C-4465-A17E-18A83E8ED2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E9D2A7-CCDB-4547-A710-59A39B045EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORM AKI &amp; AKB" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>jumlah_aki</t>
   </si>
@@ -33,38 +33,23 @@
     <t>desa_id</t>
   </si>
   <si>
-    <t>53.06.13.2021</t>
-  </si>
-  <si>
-    <t>53.06.13.2020</t>
-  </si>
-  <si>
-    <t>53.06.13.2019</t>
-  </si>
-  <si>
-    <t>53.06.13.2018</t>
-  </si>
-  <si>
-    <t>53.06.13.2017</t>
-  </si>
-  <si>
-    <t>53.06.13.2016</t>
-  </si>
-  <si>
-    <t>53.06.13.2015</t>
-  </si>
-  <si>
-    <t>53.06.13.2014</t>
+    <t>53.06.13.2001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,17 +434,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -470,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -481,9 +466,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -492,9 +477,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>343</v>
@@ -503,9 +488,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>6</v>
@@ -514,9 +499,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>23</v>
@@ -525,9 +510,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -536,9 +521,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -547,9 +532,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -559,6 +544,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -569,7 +555,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -581,7 +567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>